<commit_message>
Equip pref transfer calcualtion
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/src/Test Data/eResidue_eDocs_TestCase_result.xlsx
+++ b/eResidue_CV_eDocs/src/Test Data/eResidue_eDocs_TestCase_result.xlsx
@@ -4980,8 +4980,8 @@
       <c r="AN42" s="34" t="n">
         <v>0.0012000096030533314</v>
       </c>
-      <c r="AO42" s="34" t="e">
-        <v>#DIV/0!</v>
+      <c r="AO42" s="34" t="n">
+        <v>599.9999389648438</v>
       </c>
       <c r="AP42" s="21"/>
     </row>
@@ -5075,8 +5075,8 @@
       <c r="AN43" s="34" t="n">
         <v>4.0000322042033076E-4</v>
       </c>
-      <c r="AO43" s="34" t="e">
-        <v>#DIV/0!</v>
+      <c r="AO43" s="34" t="n">
+        <v>66.66667175292969</v>
       </c>
       <c r="AP43" s="21"/>
     </row>
@@ -5148,8 +5148,8 @@
       <c r="AN44" s="34" t="n">
         <v>4.0000322042033076E-4</v>
       </c>
-      <c r="AO44" s="34" t="e">
-        <v>#DIV/0!</v>
+      <c r="AO44" s="34" t="n">
+        <v>166.6666717529297</v>
       </c>
       <c r="AP44" s="21"/>
     </row>

</xml_diff>